<commit_message>
[RM]Feature #82052. Fixed vulnerabilities
Change-Id: I49b7a4922f829863c3d711a2c02e66f5d9498706
</commit_message>
<xml_diff>
--- a/BackEnd/Core/sailfish-core/src/test/resources/aml/iomatrix/XLSXwithformuladata.xlsx
+++ b/BackEnd/Core/sailfish-core/src/test/resources/aml/iomatrix/XLSXwithformuladata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,9 +22,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -109,7 +110,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -122,11 +123,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -134,18 +135,14 @@
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -211,19 +208,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.2295918367347"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,9 +604,9 @@
         <f aca="false">SIN(G11)</f>
         <v>-0.961397491879557</v>
       </c>
-      <c r="H12" s="3" t="str">
-        <f aca="false">DOLLAR(H1,B1)</f>
-        <v>$8.00</v>
+      <c r="H12" s="3" t="n">
+        <f aca="false">ABS(H1)</f>
+        <v>8</v>
       </c>
       <c r="I12" s="3" t="n">
         <f aca="false">AND(I2&gt;J3,I6&gt;J8)</f>
@@ -623,7 +620,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.786805555555556" right="0.786805555555556" top="1.05277777777778" bottom="1.05277777777778" header="0.786805555555556" footer="0.786805555555556"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -632,20 +629,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="n">
@@ -676,11 +670,11 @@
         <f aca="false">SIN(Sheet1!G9)</f>
         <v>0.650287840157117</v>
       </c>
-      <c r="H1" s="3" t="str">
-        <f aca="false">DOLLAR(Sheet1!F3,Sheet1!B1)</f>
-        <v>$8.00</v>
-      </c>
-      <c r="I1" s="6" t="n">
+      <c r="H1" s="3" t="n">
+        <f aca="false">ABS(Sheet1!F3)</f>
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="n">
         <f aca="false">AND(Sheet1!D2&gt;Sheet1!C2,Sheet1!E4&gt;Sheet1!G6)</f>
         <v>0</v>
       </c>
@@ -692,7 +686,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>